<commit_message>
executar códigos do Supplement
</commit_message>
<xml_diff>
--- a/Biostar_Catalogue/output_files/BrightStarMultiple/csv/query_around_por_estrela.xlsx
+++ b/Biostar_Catalogue/output_files/BrightStarMultiple/csv/query_around_por_estrela.xlsx
@@ -1054,48 +1054,48 @@
     <t>HD 74535</t>
   </si>
   <si>
+    <t>HD 116072</t>
+  </si>
+  <si>
+    <t>HD 116087</t>
+  </si>
+  <si>
+    <t>HD 140483</t>
+  </si>
+  <si>
+    <t>HD 140484</t>
+  </si>
+  <si>
+    <t>HD 173087</t>
+  </si>
+  <si>
+    <t>HD 173607</t>
+  </si>
+  <si>
+    <t>HD 173608</t>
+  </si>
+  <si>
+    <t>HD 186901</t>
+  </si>
+  <si>
+    <t>HD 201091</t>
+  </si>
+  <si>
+    <t>HD 201092</t>
+  </si>
+  <si>
+    <t>HD 212697</t>
+  </si>
+  <si>
+    <t>HD 212698</t>
+  </si>
+  <si>
+    <t>HD 66006</t>
+  </si>
+  <si>
     <t>HD 7788</t>
   </si>
   <si>
-    <t>HD 116072</t>
-  </si>
-  <si>
-    <t>HD 116087</t>
-  </si>
-  <si>
-    <t>HD 140483</t>
-  </si>
-  <si>
-    <t>HD 140484</t>
-  </si>
-  <si>
-    <t>HD 173087</t>
-  </si>
-  <si>
-    <t>HD 173607</t>
-  </si>
-  <si>
-    <t>HD 173608</t>
-  </si>
-  <si>
-    <t>HD 186901</t>
-  </si>
-  <si>
-    <t>HD 201091</t>
-  </si>
-  <si>
-    <t>HD 201092</t>
-  </si>
-  <si>
-    <t>HD 212697</t>
-  </si>
-  <si>
-    <t>HD 212698</t>
-  </si>
-  <si>
-    <t>HD 66006</t>
-  </si>
-  <si>
     <t>HD 135734</t>
   </si>
   <si>
@@ -1111,42 +1111,42 @@
     <t>HD 155886</t>
   </si>
   <si>
+    <t>HD 183914</t>
+  </si>
+  <si>
+    <t>HD 36486</t>
+  </si>
+  <si>
     <t>HD 108248</t>
   </si>
   <si>
-    <t>HD 183914</t>
-  </si>
-  <si>
-    <t>HD 36486</t>
+    <t>HD 108925</t>
   </si>
   <si>
     <t>HD 108249</t>
   </si>
   <si>
-    <t>HD 108925</t>
-  </si>
-  <si>
     <t>HD 147933</t>
   </si>
   <si>
     <t>HD 147934</t>
   </si>
   <si>
+    <t>HD 145501</t>
+  </si>
+  <si>
+    <t>HD 145502</t>
+  </si>
+  <si>
+    <t>HD 186408</t>
+  </si>
+  <si>
+    <t>HD 186427</t>
+  </si>
+  <si>
     <t>HD 108250</t>
   </si>
   <si>
-    <t>HD 145501</t>
-  </si>
-  <si>
-    <t>HD 145502</t>
-  </si>
-  <si>
-    <t>HD 186408</t>
-  </si>
-  <si>
-    <t>HD 186427</t>
-  </si>
-  <si>
     <t>HD 183912</t>
   </si>
   <si>
@@ -1162,15 +1162,15 @@
     <t>HD 61555</t>
   </si>
   <si>
+    <t>HD 61556</t>
+  </si>
+  <si>
     <t>HD 128620</t>
   </si>
   <si>
     <t>HD 128621</t>
   </si>
   <si>
-    <t>HD 61556</t>
-  </si>
-  <si>
     <t>HD 144668</t>
   </si>
   <si>
@@ -1189,13 +1189,13 @@
     <t>HD 36960</t>
   </si>
   <si>
+    <t>HD 25638</t>
+  </si>
+  <si>
     <t>HD 163755</t>
   </si>
   <si>
     <t>HD 163756</t>
-  </si>
-  <si>
-    <t>HD 25638</t>
   </si>
   <si>
     <t>HD 36861</t>
@@ -4435,7 +4435,7 @@
         <v>358</v>
       </c>
       <c r="B359">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="360" spans="1:2">
@@ -4499,7 +4499,7 @@
         <v>366</v>
       </c>
       <c r="B367">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="368" spans="1:2">
@@ -4523,7 +4523,7 @@
         <v>369</v>
       </c>
       <c r="B370">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="371" spans="1:2">
@@ -4563,7 +4563,7 @@
         <v>374</v>
       </c>
       <c r="B375">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="376" spans="1:2">
@@ -4579,7 +4579,7 @@
         <v>376</v>
       </c>
       <c r="B377">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="378" spans="1:2">
@@ -4627,7 +4627,7 @@
         <v>382</v>
       </c>
       <c r="B383">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="384" spans="1:2">
@@ -4635,7 +4635,7 @@
         <v>383</v>
       </c>
       <c r="B384">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="385" spans="1:2">
@@ -4699,7 +4699,7 @@
         <v>391</v>
       </c>
       <c r="B392">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="393" spans="1:2">
@@ -4707,7 +4707,7 @@
         <v>392</v>
       </c>
       <c r="B393">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="394" spans="1:2">
@@ -4715,7 +4715,7 @@
         <v>393</v>
       </c>
       <c r="B394">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="395" spans="1:2">

</xml_diff>